<commit_message>
GPLIM-3189 Don't use exceptions for flow control. Improve readability of error messages including pluralization and punctuation.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/manifest-upload/empty-manifest.xlsx
+++ b/mercury/src/test/resources/testdata/manifest-upload/empty-manifest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940"/>
+    <workbookView xWindow="13080" yWindow="6740" windowWidth="24480" windowHeight="14940"/>
   </bookViews>
   <sheets>
     <sheet name="Buick Example" sheetId="2" r:id="rId1"/>
@@ -36,17 +36,17 @@
     <t>Visit</t>
   </si>
   <si>
-    <t>T/N</t>
+    <t>Specimen_Number</t>
   </si>
   <si>
-    <t>Sample ID</t>
+    <t>SAMPLE_TYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -58,8 +58,15 @@
       <name val="MS Sans Serif"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +85,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -91,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -106,6 +119,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +524,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -521,8 +537,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -537,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>